<commit_message>
Added max net gamma to HistGammaSim_MT.py
</commit_message>
<xml_diff>
--- a/Biotechs.xlsx
+++ b/Biotechs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/simondyates/Dropbox/DataSci/PycharmProjects/EqOptions/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6515D8C0-1AFA-A045-94C2-3B9DC41F1CF7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C14F307D-FE10-3241-99E4-F6CF5310B706}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20360" yWindow="5400" windowWidth="28040" windowHeight="17440" xr2:uid="{355B3AE8-A29C-9044-A1A2-D371B9E27CB4}"/>
+    <workbookView xWindow="8680" yWindow="3620" windowWidth="28040" windowHeight="17440" xr2:uid="{355B3AE8-A29C-9044-A1A2-D371B9E27CB4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1126" uniqueCount="886">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1134" uniqueCount="891">
   <si>
     <t>Symbol</t>
   </si>
@@ -2692,6 +2692,21 @@
   </si>
   <si>
     <t>558.18M</t>
+  </si>
+  <si>
+    <t>ZGNX</t>
+  </si>
+  <si>
+    <t>VXRT</t>
+  </si>
+  <si>
+    <t>BIIB</t>
+  </si>
+  <si>
+    <t>SYNS</t>
+  </si>
+  <si>
+    <t>(manually added)</t>
   </si>
 </sst>
 </file>
@@ -2772,7 +2787,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -2785,6 +2800,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="10" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="10" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -3100,10 +3116,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EC32BEBF-C621-AC4F-AA20-F6D5B858467B}">
-  <dimension ref="A1:J257"/>
+  <dimension ref="A1:J261"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
-      <selection activeCell="A102" sqref="A102"/>
+    <sheetView tabSelected="1" topLeftCell="A227" workbookViewId="0">
+      <selection activeCell="B261" sqref="B261"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -10794,6 +10810,38 @@
         <v>18</v>
       </c>
       <c r="J257" s="4"/>
+    </row>
+    <row r="258" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+      <c r="A258" t="s">
+        <v>886</v>
+      </c>
+      <c r="B258" s="12" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="259" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+      <c r="A259" t="s">
+        <v>887</v>
+      </c>
+      <c r="B259" s="12" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="260" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+      <c r="A260" t="s">
+        <v>888</v>
+      </c>
+      <c r="B260" s="12" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="261" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+      <c r="A261" t="s">
+        <v>889</v>
+      </c>
+      <c r="B261" s="12" t="s">
+        <v>890</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>